<commit_message>
just reran some stuff
</commit_message>
<xml_diff>
--- a/fall22_salary_review/position_counts.xlsx
+++ b/fall22_salary_review/position_counts.xlsx
@@ -1,91 +1,114 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5f55ed08a9185297/Documents/GitHub/dbk_datadesk/fall22_salary_review/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="17" documentId="11_F606F024009966FD589439C3AF7F04939259993F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07AF6B0A-879A-455D-8D53-CEBB4A062E4E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t xml:space="preserve">division</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exempt Contingent II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exempt Regular</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-Tenured, Non-Regular Faculty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-Tenured, Term. Contr. Faculty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-Tenured,Cont. Contr. Faculty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nonexempt Contingent II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nonexempt Regular</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tenure Track Faculty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tenured Faculty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A. James Clark School of Engineering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">College of Agriculture &amp; Natural Resources</t>
-  </si>
-  <si>
-    <t xml:space="preserve">College of Arts &amp; Humanities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">College of Behavioral &amp; Social Sciences</t>
-  </si>
-  <si>
-    <t xml:space="preserve">College of Computer, Math &amp; Natural Sciences</t>
-  </si>
-  <si>
-    <t xml:space="preserve">College of Education</t>
-  </si>
-  <si>
-    <t xml:space="preserve">College of Information Studies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Philip Merrill College of Journalism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Robert H. Smith School of Business</t>
-  </si>
-  <si>
-    <t xml:space="preserve">School of Architecture, Planning, &amp; Preservation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">School of Public Health</t>
-  </si>
-  <si>
-    <t xml:space="preserve">School of Public Policy</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+  <si>
+    <t>division</t>
+  </si>
+  <si>
+    <t>Exempt Contingent II</t>
+  </si>
+  <si>
+    <t>Exempt Regular</t>
+  </si>
+  <si>
+    <t>Non-Tenured, Non-Regular Faculty</t>
+  </si>
+  <si>
+    <t>Non-Tenured, Term. Contr. Faculty</t>
+  </si>
+  <si>
+    <t>Non-Tenured,Cont. Contr. Faculty</t>
+  </si>
+  <si>
+    <t>Nonexempt Contingent II</t>
+  </si>
+  <si>
+    <t>Nonexempt Regular</t>
+  </si>
+  <si>
+    <t>Tenure Track Faculty</t>
+  </si>
+  <si>
+    <t>Tenured Faculty</t>
+  </si>
+  <si>
+    <t>A. James Clark School of Engineering</t>
+  </si>
+  <si>
+    <t>College of Agriculture &amp; Natural Resources</t>
+  </si>
+  <si>
+    <t>College of Arts &amp; Humanities</t>
+  </si>
+  <si>
+    <t>College of Behavioral &amp; Social Sciences</t>
+  </si>
+  <si>
+    <t>College of Computer, Math &amp; Natural Sciences</t>
+  </si>
+  <si>
+    <t>College of Education</t>
+  </si>
+  <si>
+    <t>College of Information Studies</t>
+  </si>
+  <si>
+    <t>Philip Merrill College of Journalism</t>
+  </si>
+  <si>
+    <t>Robert H. Smith School of Business</t>
+  </si>
+  <si>
+    <t>School of Architecture, Planning, &amp; Preservation</t>
+  </si>
+  <si>
+    <t>School of Public Health</t>
+  </si>
+  <si>
+    <t>School of Public Policy</t>
+  </si>
+  <si>
+    <t>All Colleges</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -121,7 +144,20 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -402,14 +438,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="41.36328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,370 +482,400 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>2</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>217</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>85</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>47</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>302</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>3</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2">
         <v>28</v>
       </c>
-      <c r="I2" t="n">
+      <c r="I2">
         <v>27</v>
       </c>
-      <c r="J2" t="n">
+      <c r="J2">
         <v>213</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>36</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>118</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>14</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>30</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>179</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>34</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3">
         <v>130</v>
       </c>
-      <c r="I3" t="n">
+      <c r="I3">
         <v>58</v>
       </c>
-      <c r="J3" t="n">
+      <c r="J3">
         <v>124</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>6</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>167</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>60</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>226</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>106</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>2</v>
       </c>
-      <c r="H4" t="n">
+      <c r="H4">
         <v>22</v>
       </c>
-      <c r="I4" t="n">
+      <c r="I4">
         <v>44</v>
       </c>
-      <c r="J4" t="n">
+      <c r="J4">
         <v>242</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5"/>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>127</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>34</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5">
         <v>53</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5">
         <v>238</v>
       </c>
-      <c r="G5"/>
-      <c r="H5" t="n">
+      <c r="H5">
         <v>15</v>
       </c>
-      <c r="I5" t="n">
+      <c r="I5">
         <v>34</v>
       </c>
-      <c r="J5" t="n">
+      <c r="J5">
         <v>153</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B6"/>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>238</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>45</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6">
         <v>99</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6">
         <v>688</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>2</v>
       </c>
-      <c r="H6" t="n">
+      <c r="H6">
         <v>49</v>
       </c>
-      <c r="I6" t="n">
+      <c r="I6">
         <v>74</v>
       </c>
-      <c r="J6" t="n">
+      <c r="J6">
         <v>344</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>47</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>47</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7">
         <v>10</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7">
         <v>119</v>
       </c>
-      <c r="G7"/>
-      <c r="H7" t="n">
+      <c r="H7">
         <v>7</v>
       </c>
-      <c r="I7" t="n">
+      <c r="I7">
         <v>13</v>
       </c>
-      <c r="J7" t="n">
+      <c r="J7">
         <v>65</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>2</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8">
         <v>44</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8">
         <v>28</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8">
         <v>18</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F8">
         <v>14</v>
       </c>
-      <c r="G8"/>
-      <c r="H8" t="n">
+      <c r="H8">
         <v>8</v>
       </c>
-      <c r="I8" t="n">
+      <c r="I8">
         <v>20</v>
       </c>
-      <c r="J8" t="n">
+      <c r="J8">
         <v>19</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B9"/>
-      <c r="C9" t="n">
+      <c r="C9">
         <v>18</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9">
         <v>38</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9">
         <v>19</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F9">
         <v>5</v>
       </c>
-      <c r="G9"/>
-      <c r="H9" t="n">
+      <c r="H9">
         <v>1</v>
       </c>
-      <c r="I9" t="n">
+      <c r="I9">
         <v>3</v>
       </c>
-      <c r="J9" t="n">
+      <c r="J9">
         <v>11</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>2</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10">
         <v>152</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10">
         <v>34</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10">
         <v>32</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F10">
         <v>45</v>
       </c>
-      <c r="G10"/>
-      <c r="H10" t="n">
+      <c r="H10">
         <v>7</v>
       </c>
-      <c r="I10" t="n">
+      <c r="I10">
         <v>18</v>
       </c>
-      <c r="J10" t="n">
+      <c r="J10">
         <v>70</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>2</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11">
         <v>16</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11">
         <v>26</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E11">
         <v>10</v>
       </c>
-      <c r="F11" t="n">
+      <c r="F11">
         <v>28</v>
       </c>
-      <c r="G11"/>
-      <c r="H11" t="n">
+      <c r="H11">
         <v>3</v>
       </c>
-      <c r="I11" t="n">
+      <c r="I11">
         <v>6</v>
       </c>
-      <c r="J11" t="n">
+      <c r="J11">
         <v>22</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C12">
         <v>49</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D12">
         <v>28</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E12">
         <v>18</v>
       </c>
-      <c r="F12" t="n">
+      <c r="F12">
         <v>69</v>
       </c>
-      <c r="G12"/>
-      <c r="H12" t="n">
+      <c r="H12">
         <v>6</v>
       </c>
-      <c r="I12" t="n">
+      <c r="I12">
         <v>16</v>
       </c>
-      <c r="J12" t="n">
+      <c r="J12">
         <v>52</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>21</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C13">
         <v>32</v>
       </c>
-      <c r="D13" t="n">
+      <c r="D13">
         <v>39</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E13">
         <v>3</v>
       </c>
-      <c r="F13" t="n">
+      <c r="F13">
         <v>33</v>
       </c>
-      <c r="G13"/>
-      <c r="H13" t="n">
+      <c r="H13">
         <v>5</v>
       </c>
-      <c r="I13" t="n">
+      <c r="I13">
         <v>6</v>
       </c>
-      <c r="J13" t="n">
+      <c r="J13">
         <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <f>SUM(B2:B13)</f>
+        <v>53</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:J14" si="0">SUM(C2:C13)</f>
+        <v>1225</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>478</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>565</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>1826</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>281</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>319</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>1332</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>